<commit_message>
Primeira distribuição do roteirizador em produção
</commit_message>
<xml_diff>
--- a/solver_input.xlsx
+++ b/solver_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\waljo\projetos\roteirizador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E339D2AB-22E4-4487-AC9C-BA79EC4EAF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FC5279-CF0A-40B9-85B1-8B1380BB2ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-135" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>SOLVER DE DISTRIBUIÇÃO DE PAX</t>
   </si>
@@ -304,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -320,13 +320,10 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -338,6 +335,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,7 +547,7 @@
   <dimension ref="B1:H57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -550,7 +560,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="8"/>
@@ -562,12 +572,12 @@
     </row>
     <row r="2" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -587,15 +597,15 @@
     </row>
     <row r="6" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -607,12 +617,12 @@
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -622,10 +632,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
@@ -635,10 +645,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -648,25 +658,23 @@
         <v>3</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.2986111111111111</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12"/>
+      <c r="C12" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
@@ -676,62 +684,64 @@
         <v>3</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
+      <c r="C14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="19">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="19">
         <v>0.30555555555555558</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="5">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
+      <c r="D16" s="19">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
@@ -748,97 +758,93 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="16">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="16">
+        <v>3</v>
+      </c>
+      <c r="D21" s="16">
+        <v>4</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="16">
+        <v>5</v>
+      </c>
+      <c r="D22" s="16">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0</v>
+      </c>
+      <c r="D23" s="16">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="2">
-        <v>6</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="C24" s="16">
+        <v>0</v>
+      </c>
+      <c r="D24" s="16">
+        <v>15</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="16">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="16">
+        <v>2</v>
+      </c>
+      <c r="D26" s="16">
         <v>4</v>
       </c>
-      <c r="D21" s="2">
-        <v>11</v>
-      </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2">
-        <v>15</v>
-      </c>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="2">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2">
-        <v>6</v>
-      </c>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1</v>
-      </c>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <v>24</v>
-      </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2">
-        <v>3</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -939,18 +945,18 @@
     </row>
     <row r="44" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="12"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="11"/>
     </row>
     <row r="46" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C46" s="8"/>
@@ -961,7 +967,7 @@
       <c r="H46" s="8"/>
     </row>
     <row r="47" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="8"/>
@@ -972,7 +978,7 @@
       <c r="H47" s="8"/>
     </row>
     <row r="48" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C48" s="8"/>
@@ -983,7 +989,7 @@
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C49" s="8"/>
@@ -994,7 +1000,7 @@
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C50" s="8"/>
@@ -1005,7 +1011,7 @@
       <c r="H50" s="8"/>
     </row>
     <row r="51" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
+      <c r="B51" s="7"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
@@ -1014,7 +1020,7 @@
       <c r="H51" s="8"/>
     </row>
     <row r="52" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C52" s="8"/>
@@ -1025,7 +1031,7 @@
       <c r="H52" s="8"/>
     </row>
     <row r="53" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C53" s="8"/>
@@ -1036,7 +1042,7 @@
       <c r="H53" s="8"/>
     </row>
     <row r="54" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C54" s="8"/>
@@ -1047,7 +1053,7 @@
       <c r="H54" s="8"/>
     </row>
     <row r="55" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C55" s="8"/>
@@ -1058,7 +1064,7 @@
       <c r="H55" s="8"/>
     </row>
     <row r="56" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C56" s="8"/>
@@ -1069,7 +1075,7 @@
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C57" s="8"/>
@@ -1081,6 +1087,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="B49:H49"/>
+    <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="B18:E18"/>
@@ -1097,16 +1113,6 @@
     <mergeCell ref="B52:H52"/>
     <mergeCell ref="B47:H47"/>
     <mergeCell ref="B53:H53"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="B51:H51"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="B49:H49"/>
-    <mergeCell ref="B48:H48"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" operator="equal" sqref="C4 C9:C16" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>